<commit_message>
fix some bugs(see README)
</commit_message>
<xml_diff>
--- a/dev/notes.xlsx
+++ b/dev/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myLearning\lipGroup\riverGroup\integerateOmics\lipidPathways\newInspirationWork\procedure\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C79A66-387A-45CF-A77A-C38B687C26E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4BC479-7C2E-4828-80A6-017A63DB6142}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{EE034DDF-90FE-4D0B-A13B-212579A2ECAA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="959">
   <si>
     <t>Function</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3665,9 +3665,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Rscript subgroupsSel.R -i "./branch/benchmark/input/HANlipid_tidy.csv" -d "./branch/benchmark/input/HANsampleList_lipid.CSV" -s "~/temp/" -p "~/temp/" </t>
-  </si>
-  <si>
     <t>脂质组学（MS_DIAL）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4179,6 +4176,39 @@
   </si>
   <si>
     <t>[同readingLipidData、MARpreproc的其他所有参数]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Rscript subgroupsSel.R -i "./branch/benchmark/input/HANlipid_tidy.csv" -d "./branch/benchmark/input/HANsampleList_lipid.CSV" -s "~/temp/" -p "~/temp/" </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于画circos图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Rscript correlation_main.R -i "./branch/benchmark/input/HANLipidMediator_imm_forcor.CSV" -d "./branch/benchmark/input/HANsampleList_lipmid.csv" -t "Metabolites" -l F -m 0.67 -j "./branch/benchmark/input/HANgene_tidy.CSV" -e "./branch/benchmark/input/HANsampleList.CSV" -u "RNAseq" -g 6 -k 4 -n F -s 0.4 -o "~/temp/cor_hi/" -b "hierarchical" </t>
+  </si>
+  <si>
+    <t>hierarchical</t>
+  </si>
+  <si>
+    <t>k_means</t>
+  </si>
+  <si>
+    <t>Rscript correlation_main.R -i "./testData/SVFmultiomics_210118/input/lipids.csv" -d "./testData/SVFmultiomics_210118/input/sampleList.csv" -t "Lipids" -l T -m 0.67 -j "./testData/SVFmultiomics_210118/input/RNAseq_genesymbol.csv" -e "./testData/SVFmultiomics_210118/input/sampleList.csv" -u "RNAseq" -g 7 -k 6 -n T -o "~/temp/cor_kmeans/" -b "k_means"</t>
+  </si>
+  <si>
+    <t>Rscript correlation_main.R -i "./testData/SVFmultiomics_210118/input/metabolites.csv" -d "./testData/SVFmultiomics_210118/input/sampleList.csv" -t "Metabolites" -m 0.67 -j "./testData/SVFmultiomics_210118/input/RNAseq_genesymbol.csv" -e "./testData/SVFmultiomics_210118/input/sampleList.csv" -u "RNAseq" -c 4 -f 3 -n T -o "~/temp/cor_db/" -b "DBSCAN"</t>
+  </si>
+  <si>
+    <t>DBSCAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rscript correlation_main.R -i "./testData/CerebrospinalFluid_multiomics/input/metabolites_tidy2.csv" -d "./testData/CerebrospinalFluid_multiomics/input/sampleList_lip.csv" -t "Metabolites" -m 0.67 -j "./testData/CerebrospinalFluid_multiomics/input/proteins_Depletion_tidy.csv" -e "./testData/CerebrospinalFluid_multiomics/input/sampleList_lip.csv" -u "Proteins" -p 0.55 -n F -s 0.82 -o "~/temp/cor_mcl/" -b "MCL" </t>
+  </si>
+  <si>
+    <t>MCL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4390,7 +4420,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4449,6 +4479,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4789,7 +4822,7 @@
   <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4990,10 +5023,10 @@
         <v>62</v>
       </c>
       <c r="K7" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D8" s="12" t="s">
         <v>49</v>
       </c>
@@ -5019,9 +5052,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="8" t="s">
-        <v>839</v>
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="15" t="s">
+        <v>838</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>62</v>
@@ -5033,10 +5066,10 @@
         <v>62</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>492</v>
       </c>
@@ -5096,7 +5129,7 @@
         <v>219</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -6591,8 +6624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0903CDAA-256C-4554-A139-C6A08F90034B}">
   <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6643,7 +6676,7 @@
     </row>
     <row r="2" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>486</v>
@@ -6652,27 +6685,27 @@
         <v>831</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>832</v>
+        <v>949</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>825</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="23" t="s">
         <v>829</v>
       </c>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="15" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>826</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F4" s="14" t="s">
@@ -6682,7 +6715,7 @@
         <v>219</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -6713,7 +6746,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="F7" s="6" t="s">
         <v>237</v>
@@ -6726,20 +6759,20 @@
         <v>531</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>485</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="15" t="s">
         <v>488</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="15" t="s">
         <v>529</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>945</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="D8" s="15" t="s">
+        <v>944</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>490</v>
       </c>
       <c r="G8" s="13" t="s">
@@ -6749,30 +6782,30 @@
       <c r="I8" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="24" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="8" t="s">
-        <v>946</v>
+    <row r="9" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="15" t="s">
+        <v>945</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>948</v>
-      </c>
-      <c r="J9" s="23"/>
-    </row>
-    <row r="10" spans="1:10" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+        <v>947</v>
+      </c>
+      <c r="J9" s="24"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="D10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="G10" s="15"/>
-      <c r="J10" s="23"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
@@ -6788,7 +6821,7 @@
       <c r="I11" s="6" t="s">
         <v>811</v>
       </c>
-      <c r="J11" s="23"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -6812,13 +6845,13 @@
       <c r="I12" t="s">
         <v>498</v>
       </c>
-      <c r="J12" s="23"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>496</v>
       </c>
-      <c r="J13" s="23"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
@@ -6842,14 +6875,14 @@
       <c r="I14" t="s">
         <v>497</v>
       </c>
-      <c r="J14" s="23"/>
+      <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="F15" t="s">
         <v>654</v>
       </c>
-      <c r="J15" s="23"/>
+      <c r="J15" s="24"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
@@ -6873,14 +6906,14 @@
       <c r="I16" t="s">
         <v>497</v>
       </c>
-      <c r="J16" s="23"/>
+      <c r="J16" s="24"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="F17" t="s">
         <v>504</v>
       </c>
-      <c r="J17" s="23"/>
+      <c r="J17" s="24"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
@@ -6904,14 +6937,14 @@
       <c r="I18" t="s">
         <v>497</v>
       </c>
-      <c r="J18" s="23"/>
+      <c r="J18" s="24"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="F19" t="s">
         <v>509</v>
       </c>
-      <c r="J19" s="23"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
@@ -6935,14 +6968,14 @@
       <c r="I20" t="s">
         <v>497</v>
       </c>
-      <c r="J20" s="23"/>
+      <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="F21" t="s">
         <v>513</v>
       </c>
-      <c r="J21" s="23"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
@@ -6966,14 +6999,14 @@
       <c r="I22" t="s">
         <v>497</v>
       </c>
-      <c r="J22" s="23"/>
+      <c r="J22" s="24"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="F23" t="s">
         <v>670</v>
       </c>
-      <c r="J23" s="23"/>
+      <c r="J23" s="24"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
@@ -6997,13 +7030,13 @@
       <c r="I24" t="s">
         <v>497</v>
       </c>
-      <c r="J24" s="23"/>
+      <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>515</v>
       </c>
-      <c r="J25" s="23"/>
+      <c r="J25" s="24"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
@@ -7027,13 +7060,13 @@
       <c r="I26" t="s">
         <v>497</v>
       </c>
-      <c r="J26" s="23"/>
+      <c r="J26" s="24"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>682</v>
       </c>
-      <c r="J27" s="23"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -7086,7 +7119,7 @@
       <c r="I30" t="s">
         <v>695</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="J30" s="24" t="s">
         <v>586</v>
       </c>
     </row>
@@ -7100,7 +7133,7 @@
       <c r="I31" t="s">
         <v>517</v>
       </c>
-      <c r="J31" s="23"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
@@ -7112,7 +7145,7 @@
       <c r="I32" t="s">
         <v>122</v>
       </c>
-      <c r="J32" s="23"/>
+      <c r="J32" s="24"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
@@ -7124,7 +7157,7 @@
       <c r="I33" t="s">
         <v>537</v>
       </c>
-      <c r="J33" s="23"/>
+      <c r="J33" s="24"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F34" s="12" t="s">
@@ -7137,7 +7170,7 @@
       <c r="I34" s="13" t="s">
         <v>542</v>
       </c>
-      <c r="J34" s="23"/>
+      <c r="J34" s="24"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F35" s="10" t="s">
@@ -7149,7 +7182,7 @@
       <c r="I35" t="s">
         <v>539</v>
       </c>
-      <c r="J35" s="23"/>
+      <c r="J35" s="24"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
@@ -7161,7 +7194,7 @@
       <c r="I36" t="s">
         <v>541</v>
       </c>
-      <c r="J36" s="23"/>
+      <c r="J36" s="24"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F37" s="6" t="s">
@@ -7174,7 +7207,7 @@
       <c r="I37" s="6" t="s">
         <v>811</v>
       </c>
-      <c r="J37" s="23"/>
+      <c r="J37" s="24"/>
     </row>
     <row r="38" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
@@ -7198,7 +7231,7 @@
       <c r="I38" t="s">
         <v>563</v>
       </c>
-      <c r="J38" s="23"/>
+      <c r="J38" s="24"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
@@ -7210,7 +7243,7 @@
       <c r="I39" t="s">
         <v>65</v>
       </c>
-      <c r="J39" s="23"/>
+      <c r="J39" s="24"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -7234,13 +7267,13 @@
       <c r="I40" t="s">
         <v>562</v>
       </c>
-      <c r="J40" s="23"/>
+      <c r="J40" s="24"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
         <v>577</v>
       </c>
-      <c r="J41" s="23"/>
+      <c r="J41" s="24"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -7264,13 +7297,13 @@
       <c r="I42" t="s">
         <v>562</v>
       </c>
-      <c r="J42" s="23"/>
+      <c r="J42" s="24"/>
     </row>
     <row r="43" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F43" t="s">
         <v>580</v>
       </c>
-      <c r="J43" s="23"/>
+      <c r="J43" s="24"/>
     </row>
     <row r="44" spans="1:10" s="9" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
@@ -7334,7 +7367,7 @@
         <v>759</v>
       </c>
       <c r="I47" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -7682,82 +7715,91 @@
         <v>440</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C71" s="19" t="s">
         <v>441</v>
       </c>
-      <c r="D71" s="19" t="s">
-        <v>853</v>
+      <c r="D71" s="20" t="s">
+        <v>852</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="F71" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="G71" s="20" t="s">
-        <v>904</v>
-      </c>
-      <c r="H71" s="20"/>
-      <c r="I71" s="20"/>
+      <c r="G71" s="21" t="s">
+        <v>903</v>
+      </c>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
     </row>
     <row r="72" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D72" s="15" t="s">
-        <v>854</v>
+      <c r="D72" s="13" t="s">
+        <v>853</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="F72" s="15" t="s">
         <v>443</v>
       </c>
-      <c r="G72" s="21"/>
-      <c r="H72" s="21"/>
-      <c r="I72" s="21"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="22"/>
+      <c r="I72" s="22"/>
     </row>
     <row r="73" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D73" s="15" t="s">
-        <v>888</v>
+      <c r="D73" s="13" t="s">
+        <v>887</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="F73" s="15" t="s">
         <v>444</v>
       </c>
-      <c r="G73" s="21"/>
-      <c r="H73" s="21"/>
-      <c r="I73" s="21"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
     </row>
     <row r="74" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D74" s="15" t="s">
-        <v>906</v>
+      <c r="D74" s="13" t="s">
+        <v>905</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="F74" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="G74" s="21"/>
-      <c r="H74" s="21"/>
-      <c r="I74" s="21"/>
-    </row>
-    <row r="75" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D75" s="15" t="s">
-        <v>928</v>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="22"/>
+    </row>
+    <row r="75" spans="1:10" s="15" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D75" s="13" t="s">
+        <v>927</v>
+      </c>
+      <c r="E75" s="15" t="s">
+        <v>950</v>
       </c>
       <c r="F75" s="15" t="s">
-        <v>842</v>
-      </c>
-      <c r="G75" s="22" t="s">
-        <v>905</v>
-      </c>
-      <c r="H75" s="22"/>
-      <c r="I75" s="22"/>
-    </row>
-    <row r="76" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>841</v>
+      </c>
+      <c r="G75" s="23" t="s">
+        <v>904</v>
+      </c>
+      <c r="H75" s="23"/>
+      <c r="I75" s="23"/>
+    </row>
+    <row r="76" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D76" s="8" t="s">
+        <v>951</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>952</v>
+      </c>
       <c r="F76" s="15" t="s">
         <v>446</v>
       </c>
@@ -7766,10 +7808,16 @@
       </c>
       <c r="H76" s="18"/>
       <c r="I76" s="18" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D77" s="8" t="s">
+        <v>954</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>953</v>
+      </c>
       <c r="F77" s="15" t="s">
         <v>447</v>
       </c>
@@ -7778,10 +7826,16 @@
       </c>
       <c r="H77" s="18"/>
       <c r="I77" s="18" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" s="15" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D78" s="8" t="s">
+        <v>955</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>956</v>
+      </c>
       <c r="F78" s="15" t="s">
         <v>448</v>
       </c>
@@ -7789,11 +7843,17 @@
         <v>219</v>
       </c>
       <c r="I78" s="15" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="79" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F79" s="8" t="s">
+      <c r="D79" s="8" t="s">
+        <v>957</v>
+      </c>
+      <c r="E79" s="15" t="s">
+        <v>958</v>
+      </c>
+      <c r="F79" s="15" t="s">
         <v>449</v>
       </c>
       <c r="G79" s="15" t="s">
@@ -7803,11 +7863,11 @@
         <v>4</v>
       </c>
       <c r="I79" s="15" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F80" s="8" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="15" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F80" s="15" t="s">
         <v>408</v>
       </c>
       <c r="G80" s="15" t="s">
@@ -7817,38 +7877,38 @@
         <v>4</v>
       </c>
       <c r="I80" s="15" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" s="15" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F81" s="15" t="s">
+        <v>844</v>
+      </c>
+      <c r="G81" s="15" t="s">
         <v>845</v>
       </c>
-      <c r="G81" s="15" t="s">
+      <c r="H81" s="15" t="s">
         <v>846</v>
       </c>
-      <c r="H81" s="15" t="s">
-        <v>847</v>
-      </c>
       <c r="I81" s="15" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F82" s="15" t="s">
+        <v>847</v>
+      </c>
+      <c r="G82" s="15" t="s">
         <v>848</v>
-      </c>
-      <c r="G82" s="15" t="s">
-        <v>849</v>
       </c>
       <c r="H82" s="15">
         <v>0.8</v>
       </c>
       <c r="I82" s="15" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" s="15" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F83" s="15" t="s">
         <v>450</v>
       </c>
@@ -7859,23 +7919,23 @@
         <v>452</v>
       </c>
     </row>
-    <row r="84" spans="1:9" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F84" s="8" t="s">
-        <v>931</v>
+    <row r="84" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F84" s="15" t="s">
+        <v>930</v>
       </c>
       <c r="G84" s="15" t="s">
         <v>219</v>
       </c>
       <c r="H84" s="15" t="s">
+        <v>931</v>
+      </c>
+      <c r="I84" s="15" t="s">
         <v>932</v>
       </c>
-      <c r="I84" s="15" t="s">
+    </row>
+    <row r="85" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F85" s="15" t="s">
         <v>933</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F85" s="8" t="s">
-        <v>934</v>
       </c>
       <c r="G85" s="15" t="s">
         <v>266</v>
@@ -7884,12 +7944,12 @@
         <v>4</v>
       </c>
       <c r="I85" s="15" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F86" s="8" t="s">
-        <v>935</v>
+        <v>936</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F86" s="15" t="s">
+        <v>934</v>
       </c>
       <c r="G86" s="15" t="s">
         <v>266</v>
@@ -7898,12 +7958,12 @@
         <v>3</v>
       </c>
       <c r="I86" s="15" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F87" s="15" t="s">
         <v>939</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F87" s="8" t="s">
-        <v>940</v>
       </c>
       <c r="G87" s="15" t="s">
         <v>322</v>
@@ -7912,21 +7972,21 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="I87" s="15" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" s="15" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
         <v>462</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>463</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="F88" s="15" t="s">
         <v>590</v>
@@ -7935,7 +7995,7 @@
         <v>219</v>
       </c>
       <c r="I88" s="15" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="89" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -7946,7 +8006,7 @@
         <v>266</v>
       </c>
       <c r="I89" s="15" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -7957,7 +8017,7 @@
         <v>266</v>
       </c>
       <c r="I90" s="15" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -7969,7 +8029,7 @@
       </c>
       <c r="H91" s="6"/>
       <c r="I91" s="6" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="92" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -7980,7 +8040,7 @@
         <v>607</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>614</v>
@@ -7997,7 +8057,7 @@
     </row>
     <row r="93" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D93" s="15" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F93" s="15" t="s">
         <v>616</v>
@@ -8006,7 +8066,7 @@
         <v>597</v>
       </c>
       <c r="I93" s="15" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8017,7 +8077,7 @@
         <v>617</v>
       </c>
       <c r="I94" s="15" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8053,7 +8113,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="98" spans="1:10" s="15" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F98" s="15" t="s">
         <v>596</v>
       </c>
@@ -8064,35 +8124,34 @@
         <v>65</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E99" s="8"/>
+        <v>907</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F99" s="6" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="G99" s="6" t="s">
         <v>220</v>
       </c>
       <c r="H99" s="6"/>
       <c r="I99" s="6" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="J99" s="1"/>
     </row>
-    <row r="100" spans="1:10" s="15" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B100" s="15" t="s">
         <v>607</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D100" s="15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F100" s="15" t="s">
         <v>217</v>
@@ -8101,7 +8160,7 @@
         <v>219</v>
       </c>
       <c r="I100" s="15" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="101" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8112,7 +8171,7 @@
         <v>266</v>
       </c>
       <c r="I101" s="15" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="102" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8123,7 +8182,7 @@
         <v>219</v>
       </c>
       <c r="I102" s="15" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="103" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8148,7 +8207,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="105" spans="1:10" s="15" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F105" s="15" t="s">
         <v>232</v>
       </c>
@@ -8159,60 +8218,59 @@
         <v>65</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E106" s="8"/>
+        <v>907</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F106" s="6" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="G106" s="6" t="s">
         <v>220</v>
       </c>
       <c r="H106" s="6"/>
       <c r="I106" s="6" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="J106" s="1"/>
     </row>
-    <row r="107" spans="1:10" s="15" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B107" s="15" t="s">
         <v>607</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D107" s="15" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="F107" s="15" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="G107" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I107" s="15" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="108" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F108" s="15" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="G108" s="15" t="s">
         <v>74</v>
       </c>
       <c r="I108" s="15" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="109" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F109" s="15" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="G109" s="15" t="s">
         <v>219</v>
@@ -8223,41 +8281,41 @@
     </row>
     <row r="110" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B110" s="15" t="s">
         <v>607</v>
       </c>
       <c r="C110" s="15" t="s">
+        <v>897</v>
+      </c>
+      <c r="D110" s="15" t="s">
         <v>898</v>
       </c>
-      <c r="D110" s="15" t="s">
-        <v>899</v>
-      </c>
       <c r="F110" s="15" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="G110" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I110" s="15" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="111" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F111" s="15" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="G111" s="15" t="s">
         <v>74</v>
       </c>
       <c r="I111" s="15" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" s="15" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F112" s="15" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="G112" s="15" t="s">
         <v>219</v>
@@ -8266,41 +8324,41 @@
         <v>65</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="8" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="15" t="s">
+        <v>917</v>
+      </c>
+      <c r="B113" s="15" t="s">
+        <v>851</v>
+      </c>
+      <c r="C113" s="15" t="s">
         <v>918</v>
       </c>
-      <c r="B113" s="15" t="s">
-        <v>852</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>919</v>
-      </c>
       <c r="D113" s="15" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F113" s="15" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G113" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I113" s="15" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" s="15" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F114" s="15" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G114" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I114" s="15" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8311,7 +8369,7 @@
         <v>266</v>
       </c>
       <c r="I115" s="15" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8322,26 +8380,26 @@
         <v>266</v>
       </c>
       <c r="I116" s="15" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F117" s="15" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="G117" s="15" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="H117" s="15">
         <v>0.6</v>
       </c>
       <c r="I117" s="15" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="118" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F118" s="15" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="G118" s="15" t="s">
         <v>266</v>
@@ -8350,18 +8408,18 @@
         <v>20</v>
       </c>
       <c r="I118" s="15" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="119" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F119" s="15" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G119" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I119" s="15" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="120" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -8398,8 +8456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B31EB-83BB-43B1-BAC3-91B270982CA0}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8467,7 +8525,7 @@
       <c r="E3" t="s">
         <v>471</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="23" t="s">
         <v>707</v>
       </c>
     </row>
@@ -8484,7 +8542,7 @@
       <c r="E4" t="s">
         <v>472</v>
       </c>
-      <c r="F4" s="22"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -8499,7 +8557,7 @@
       <c r="E5" t="s">
         <v>473</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -8517,7 +8575,7 @@
       <c r="E6" t="s">
         <v>430</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="23" t="s">
         <v>706</v>
       </c>
       <c r="G6" t="s">
@@ -8540,7 +8598,7 @@
       <c r="E7" t="s">
         <v>656</v>
       </c>
-      <c r="F7" s="22"/>
+      <c r="F7" s="23"/>
       <c r="G7" t="s">
         <v>714</v>
       </c>
@@ -8561,7 +8619,7 @@
       <c r="E8" t="s">
         <v>431</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="23" t="s">
         <v>701</v>
       </c>
     </row>
@@ -8579,7 +8637,7 @@
       <c r="E9" t="s">
         <v>432</v>
       </c>
-      <c r="F9" s="22"/>
+      <c r="F9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
@@ -8595,7 +8653,7 @@
       <c r="E10" t="s">
         <v>755</v>
       </c>
-      <c r="F10" s="22"/>
+      <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -8613,7 +8671,7 @@
       <c r="E11" t="s">
         <v>399</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="23" t="s">
         <v>708</v>
       </c>
       <c r="G11" t="s">
@@ -8633,7 +8691,7 @@
       <c r="E12" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="F12" s="22"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -8648,7 +8706,7 @@
       <c r="E13" t="s">
         <v>465</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -8663,7 +8721,7 @@
       <c r="E14" t="s">
         <v>482</v>
       </c>
-      <c r="F14" s="22"/>
+      <c r="F14" s="23"/>
       <c r="G14" t="s">
         <v>710</v>
       </c>
@@ -8681,7 +8739,7 @@
       <c r="E15" t="s">
         <v>401</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="23"/>
       <c r="G15" t="s">
         <v>704</v>
       </c>
@@ -8702,7 +8760,7 @@
       <c r="E16" t="s">
         <v>673</v>
       </c>
-      <c r="F16" s="22"/>
+      <c r="F16" s="23"/>
       <c r="G16" t="s">
         <v>716</v>
       </c>
@@ -8726,7 +8784,7 @@
       <c r="E17" t="s">
         <v>403</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="23" t="s">
         <v>709</v>
       </c>
     </row>
@@ -8743,7 +8801,7 @@
       <c r="E18" t="s">
         <v>405</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="23"/>
       <c r="G18" t="s">
         <v>702</v>
       </c>
@@ -8761,7 +8819,7 @@
       <c r="E19" t="s">
         <v>692</v>
       </c>
-      <c r="F19" s="22"/>
+      <c r="F19" s="23"/>
       <c r="G19" t="s">
         <v>701</v>
       </c>
@@ -8782,7 +8840,7 @@
       <c r="E20" t="s">
         <v>402</v>
       </c>
-      <c r="F20" s="22"/>
+      <c r="F20" s="23"/>
       <c r="G20" t="s">
         <v>704</v>
       </c>
@@ -8820,7 +8878,7 @@
       <c r="E22" t="s">
         <v>557</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="23" t="s">
         <v>818</v>
       </c>
     </row>
@@ -8837,7 +8895,7 @@
       <c r="E23" t="s">
         <v>554</v>
       </c>
-      <c r="F23" s="22"/>
+      <c r="F23" s="23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="15" t="s">
@@ -8852,7 +8910,7 @@
       <c r="E24" t="s">
         <v>558</v>
       </c>
-      <c r="F24" s="22"/>
+      <c r="F24" s="23"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
@@ -8867,7 +8925,7 @@
       <c r="E25" t="s">
         <v>559</v>
       </c>
-      <c r="F25" s="22"/>
+      <c r="F25" s="23"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -8882,7 +8940,7 @@
       <c r="E26" t="s">
         <v>561</v>
       </c>
-      <c r="F26" s="22"/>
+      <c r="F26" s="23"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -8900,7 +8958,7 @@
       <c r="E27" t="s">
         <v>430</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="23" t="s">
         <v>817</v>
       </c>
     </row>
@@ -8917,7 +8975,7 @@
       <c r="E28" t="s">
         <v>571</v>
       </c>
-      <c r="F28" s="22"/>
+      <c r="F28" s="23"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -8975,7 +9033,7 @@
       <c r="E31" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="25" t="s">
         <v>743</v>
       </c>
       <c r="H31" s="9" t="s">
@@ -8995,7 +9053,7 @@
       <c r="E32" s="17" t="s">
         <v>793</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
@@ -9010,7 +9068,7 @@
       <c r="E33" s="17" t="s">
         <v>794</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -9028,7 +9086,7 @@
       <c r="E34" s="14" t="s">
         <v>740</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="23" t="s">
         <v>742</v>
       </c>
     </row>
@@ -9045,7 +9103,7 @@
       <c r="E35" s="14" t="s">
         <v>741</v>
       </c>
-      <c r="F35" s="22"/>
+      <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -9063,7 +9121,7 @@
       <c r="E36" t="s">
         <v>642</v>
       </c>
-      <c r="F36" s="22"/>
+      <c r="F36" s="23"/>
       <c r="H36" t="s">
         <v>801</v>
       </c>
@@ -9081,7 +9139,7 @@
       <c r="E37" t="s">
         <v>643</v>
       </c>
-      <c r="F37" s="22"/>
+      <c r="F37" s="23"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -9096,7 +9154,7 @@
       <c r="E38" t="s">
         <v>644</v>
       </c>
-      <c r="F38" s="22"/>
+      <c r="F38" s="23"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -9114,7 +9172,7 @@
       <c r="E39" t="s">
         <v>775</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="F39" s="23" t="s">
         <v>773</v>
       </c>
     </row>
@@ -9131,7 +9189,7 @@
       <c r="E40" t="s">
         <v>776</v>
       </c>
-      <c r="F40" s="22"/>
+      <c r="F40" s="23"/>
       <c r="H40" s="15" t="s">
         <v>801</v>
       </c>
@@ -9149,7 +9207,7 @@
       <c r="E41" t="s">
         <v>777</v>
       </c>
-      <c r="F41" s="22"/>
+      <c r="F41" s="23"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
@@ -9164,7 +9222,7 @@
       <c r="E42" t="s">
         <v>778</v>
       </c>
-      <c r="F42" s="22"/>
+      <c r="F42" s="23"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="15" t="s">
@@ -9179,7 +9237,7 @@
       <c r="E43" t="s">
         <v>779</v>
       </c>
-      <c r="F43" s="22"/>
+      <c r="F43" s="23"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
@@ -9194,7 +9252,7 @@
       <c r="E44" t="s">
         <v>787</v>
       </c>
-      <c r="F44" s="22"/>
+      <c r="F44" s="23"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -9209,7 +9267,7 @@
       <c r="E45" t="s">
         <v>785</v>
       </c>
-      <c r="F45" s="22"/>
+      <c r="F45" s="23"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -9224,7 +9282,7 @@
       <c r="E46" t="s">
         <v>786</v>
       </c>
-      <c r="F46" s="22"/>
+      <c r="F46" s="23"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -9242,8 +9300,8 @@
       <c r="E47" t="s">
         <v>798</v>
       </c>
-      <c r="F47" s="22" t="s">
-        <v>838</v>
+      <c r="F47" s="23" t="s">
+        <v>837</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -9259,7 +9317,7 @@
       <c r="E48" t="s">
         <v>799</v>
       </c>
-      <c r="F48" s="22"/>
+      <c r="F48" s="23"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -9277,7 +9335,7 @@
       <c r="E49" t="s">
         <v>808</v>
       </c>
-      <c r="F49" s="22"/>
+      <c r="F49" s="23"/>
       <c r="H49" s="15" t="s">
         <v>801</v>
       </c>
@@ -9290,7 +9348,7 @@
         <v>457</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>458</v>
@@ -9304,7 +9362,7 @@
         <v>460</v>
       </c>
       <c r="C51" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D51" t="s">
         <v>458</v>
@@ -9329,7 +9387,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C53" t="s">
         <v>400</v>
@@ -9338,13 +9396,13 @@
         <v>458</v>
       </c>
       <c r="E53" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
       <c r="B54" s="15" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>459</v>
@@ -9353,15 +9411,15 @@
         <v>458</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B55" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>400</v>
@@ -9370,15 +9428,15 @@
         <v>458</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B56" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C56" t="s">
         <v>400</v>
@@ -9387,15 +9445,15 @@
         <v>458</v>
       </c>
       <c r="E56" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B57" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C57" t="s">
         <v>459</v>
@@ -9404,12 +9462,12 @@
         <v>458</v>
       </c>
       <c r="E57" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C58" t="s">
         <v>400</v>
@@ -9418,15 +9476,15 @@
         <v>458</v>
       </c>
       <c r="E58" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
+        <v>892</v>
+      </c>
+      <c r="B59" t="s">
         <v>893</v>
-      </c>
-      <c r="B59" t="s">
-        <v>894</v>
       </c>
       <c r="C59" t="s">
         <v>400</v>
@@ -9435,12 +9493,12 @@
         <v>458</v>
       </c>
       <c r="E59" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C60" t="s">
         <v>459</v>
@@ -9449,12 +9507,12 @@
         <v>458</v>
       </c>
       <c r="E60" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C61" t="s">
         <v>459</v>
@@ -9463,23 +9521,23 @@
         <v>458</v>
       </c>
       <c r="E61" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="65" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F11:F16"/>
+    <mergeCell ref="F17:F20"/>
+    <mergeCell ref="F8:F10"/>
     <mergeCell ref="F47:F49"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="F22:F26"/>
     <mergeCell ref="F39:F46"/>
     <mergeCell ref="F31:F33"/>
     <mergeCell ref="F34:F38"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F11:F16"/>
-    <mergeCell ref="F17:F20"/>
-    <mergeCell ref="F8:F10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9709,18 +9767,18 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>832</v>
+      </c>
+      <c r="B23" t="s">
         <v>833</v>
       </c>
-      <c r="B23" t="s">
-        <v>834</v>
-      </c>
       <c r="D23" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
   </sheetData>
@@ -9833,10 +9891,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>941</v>
+      </c>
+      <c r="B2" t="s">
         <v>942</v>
-      </c>
-      <c r="B2" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9916,10 +9974,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>94</v>
       </c>
       <c r="C2" t="s">
@@ -9945,8 +10003,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="D3" t="s">
         <v>38</v>
       </c>
@@ -9967,8 +10025,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="D4" t="s">
         <v>40</v>
       </c>
@@ -9980,8 +10038,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="D5" t="s">
         <v>44</v>
       </c>
@@ -10002,8 +10060,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="D6" t="s">
         <v>175</v>
       </c>
@@ -10021,8 +10079,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
       <c r="D7" t="s">
         <v>46</v>
       </c>
@@ -10039,8 +10097,8 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
       <c r="D8" t="s">
         <v>48</v>
       </c>
@@ -10061,8 +10119,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
       <c r="D9" t="s">
         <v>49</v>
       </c>
@@ -10074,8 +10132,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
       <c r="C10" t="s">
         <v>51</v>
       </c>
@@ -10084,8 +10142,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
       <c r="C11" t="s">
         <v>66</v>
       </c>
@@ -10094,15 +10152,15 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
       <c r="D12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
       <c r="D13" t="s">
         <v>48</v>
       </c>
@@ -10123,8 +10181,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
       <c r="C14" t="s">
         <v>69</v>
       </c>
@@ -10133,15 +10191,15 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
       <c r="D15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
       <c r="D16" t="s">
         <v>48</v>
       </c>
@@ -10162,8 +10220,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
       <c r="D17" t="s">
         <v>199</v>
       </c>
@@ -10184,8 +10242,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
       <c r="C18" t="s">
         <v>76</v>
       </c>
@@ -10194,15 +10252,15 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="D19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
       <c r="D20" t="s">
         <v>48</v>
       </c>
@@ -10219,8 +10277,8 @@
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
       <c r="C21" t="s">
         <v>201</v>
       </c>
@@ -10229,15 +10287,15 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
       <c r="D22" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
       <c r="D23" t="s">
         <v>48</v>
       </c>
@@ -10254,8 +10312,8 @@
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
       <c r="D24" t="s">
         <v>81</v>
       </c>
@@ -10272,15 +10330,15 @@
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
       <c r="D25" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="25" t="s">
+      <c r="A26" s="23"/>
+      <c r="B26" s="26" t="s">
         <v>98</v>
       </c>
       <c r="C26" t="s">
@@ -10306,8 +10364,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="25"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="26"/>
       <c r="D27" t="s">
         <v>38</v>
       </c>
@@ -10328,8 +10386,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="26"/>
       <c r="D28" t="s">
         <v>40</v>
       </c>
@@ -10341,8 +10399,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="25"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="26"/>
       <c r="D29" t="s">
         <v>44</v>
       </c>
@@ -10363,8 +10421,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="25"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="26"/>
       <c r="D30" t="s">
         <v>45</v>
       </c>
@@ -10382,8 +10440,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="26"/>
       <c r="D31" t="s">
         <v>46</v>
       </c>
@@ -10400,8 +10458,8 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="25"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="26"/>
       <c r="D32" t="s">
         <v>48</v>
       </c>
@@ -10422,8 +10480,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="26"/>
       <c r="D33" t="s">
         <v>49</v>
       </c>
@@ -10435,8 +10493,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="25"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="26"/>
       <c r="C34" t="s">
         <v>51</v>
       </c>
@@ -10445,8 +10503,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="25"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="26"/>
       <c r="C35" t="s">
         <v>58</v>
       </c>
@@ -10455,15 +10513,15 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="25"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="26"/>
       <c r="D36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="25"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="26"/>
       <c r="D37" t="s">
         <v>61</v>
       </c>
@@ -10480,8 +10538,8 @@
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="25"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="26"/>
       <c r="D38" t="s">
         <v>48</v>
       </c>
@@ -10502,8 +10560,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="25"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="26"/>
       <c r="C39" t="s">
         <v>66</v>
       </c>
@@ -10512,15 +10570,15 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="25"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="26"/>
       <c r="D40" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="25"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="26"/>
       <c r="D41" t="s">
         <v>48</v>
       </c>
@@ -10541,8 +10599,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="25"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="26"/>
       <c r="C42" t="s">
         <v>69</v>
       </c>
@@ -10551,15 +10609,15 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="25"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="26"/>
       <c r="D43" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="25"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="26"/>
       <c r="D44" t="s">
         <v>48</v>
       </c>
@@ -10580,8 +10638,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="26"/>
       <c r="D45" t="s">
         <v>199</v>
       </c>
@@ -10602,8 +10660,8 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="25"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="26"/>
       <c r="C46" t="s">
         <v>76</v>
       </c>
@@ -10612,15 +10670,15 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="25"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="26"/>
       <c r="D47" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="25"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="26"/>
       <c r="D48" t="s">
         <v>48</v>
       </c>
@@ -10637,8 +10695,8 @@
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="25"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="26"/>
       <c r="C49" t="s">
         <v>201</v>
       </c>
@@ -10647,15 +10705,15 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="25"/>
+      <c r="A50" s="23"/>
+      <c r="B50" s="26"/>
       <c r="D50" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="25"/>
+      <c r="A51" s="23"/>
+      <c r="B51" s="26"/>
       <c r="D51" t="s">
         <v>48</v>
       </c>
@@ -10672,8 +10730,8 @@
       <c r="I51" s="5"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="25"/>
+      <c r="A52" s="23"/>
+      <c r="B52" s="26"/>
       <c r="D52" t="s">
         <v>81</v>
       </c>
@@ -10690,15 +10748,15 @@
       <c r="I52" s="5"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="25"/>
+      <c r="A53" s="23"/>
+      <c r="B53" s="26"/>
       <c r="D53" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="22" t="s">
+      <c r="A54" s="23"/>
+      <c r="B54" s="23" t="s">
         <v>101</v>
       </c>
       <c r="C54" t="s">
@@ -10724,8 +10782,8 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="22"/>
-      <c r="B55" s="22"/>
+      <c r="A55" s="23"/>
+      <c r="B55" s="23"/>
       <c r="D55" t="s">
         <v>38</v>
       </c>
@@ -10746,8 +10804,8 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="22"/>
-      <c r="B56" s="22"/>
+      <c r="A56" s="23"/>
+      <c r="B56" s="23"/>
       <c r="D56" t="s">
         <v>40</v>
       </c>
@@ -10759,8 +10817,8 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="22"/>
-      <c r="B57" s="22"/>
+      <c r="A57" s="23"/>
+      <c r="B57" s="23"/>
       <c r="D57" t="s">
         <v>44</v>
       </c>
@@ -10781,8 +10839,8 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
-      <c r="B58" s="22"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="23"/>
       <c r="D58" t="s">
         <v>45</v>
       </c>
@@ -10800,8 +10858,8 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="B59" s="22"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="23"/>
       <c r="D59" t="s">
         <v>46</v>
       </c>
@@ -10818,8 +10876,8 @@
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
       <c r="D60" t="s">
         <v>48</v>
       </c>
@@ -10840,8 +10898,8 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="22"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="23"/>
       <c r="D61" t="s">
         <v>49</v>
       </c>
@@ -10853,8 +10911,8 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
-      <c r="B62" s="22"/>
+      <c r="A62" s="23"/>
+      <c r="B62" s="23"/>
       <c r="C62" t="s">
         <v>51</v>
       </c>
@@ -10863,8 +10921,8 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="22"/>
+      <c r="A63" s="23"/>
+      <c r="B63" s="23"/>
       <c r="C63" t="s">
         <v>58</v>
       </c>
@@ -10873,15 +10931,15 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="22"/>
-      <c r="B64" s="22"/>
+      <c r="A64" s="23"/>
+      <c r="B64" s="23"/>
       <c r="D64" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="22"/>
-      <c r="B65" s="22"/>
+      <c r="A65" s="23"/>
+      <c r="B65" s="23"/>
       <c r="D65" t="s">
         <v>61</v>
       </c>
@@ -10898,8 +10956,8 @@
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="22"/>
-      <c r="B66" s="22"/>
+      <c r="A66" s="23"/>
+      <c r="B66" s="23"/>
       <c r="D66" t="s">
         <v>48</v>
       </c>
@@ -10920,8 +10978,8 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="22"/>
-      <c r="B67" s="22"/>
+      <c r="A67" s="23"/>
+      <c r="B67" s="23"/>
       <c r="C67" t="s">
         <v>66</v>
       </c>
@@ -10930,15 +10988,15 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="22"/>
-      <c r="B68" s="22"/>
+      <c r="A68" s="23"/>
+      <c r="B68" s="23"/>
       <c r="D68" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="22"/>
-      <c r="B69" s="22"/>
+      <c r="A69" s="23"/>
+      <c r="B69" s="23"/>
       <c r="D69" t="s">
         <v>48</v>
       </c>
@@ -10959,8 +11017,8 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
+      <c r="A70" s="23"/>
+      <c r="B70" s="23"/>
       <c r="C70" t="s">
         <v>69</v>
       </c>
@@ -10969,15 +11027,15 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="22"/>
-      <c r="B71" s="22"/>
+      <c r="A71" s="23"/>
+      <c r="B71" s="23"/>
       <c r="D71" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="22"/>
-      <c r="B72" s="22"/>
+      <c r="A72" s="23"/>
+      <c r="B72" s="23"/>
       <c r="D72" t="s">
         <v>48</v>
       </c>
@@ -10998,8 +11056,8 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="22"/>
-      <c r="B73" s="22"/>
+      <c r="A73" s="23"/>
+      <c r="B73" s="23"/>
       <c r="D73" t="s">
         <v>199</v>
       </c>
@@ -11020,8 +11078,8 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="22"/>
-      <c r="B74" s="22"/>
+      <c r="A74" s="23"/>
+      <c r="B74" s="23"/>
       <c r="C74" t="s">
         <v>76</v>
       </c>
@@ -11030,15 +11088,15 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="22"/>
-      <c r="B75" s="22"/>
+      <c r="A75" s="23"/>
+      <c r="B75" s="23"/>
       <c r="D75" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="22"/>
-      <c r="B76" s="22"/>
+      <c r="A76" s="23"/>
+      <c r="B76" s="23"/>
       <c r="D76" t="s">
         <v>48</v>
       </c>
@@ -11055,8 +11113,8 @@
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="22"/>
-      <c r="B77" s="22"/>
+      <c r="A77" s="23"/>
+      <c r="B77" s="23"/>
       <c r="C77" t="s">
         <v>201</v>
       </c>
@@ -11065,15 +11123,15 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="22"/>
-      <c r="B78" s="22"/>
+      <c r="A78" s="23"/>
+      <c r="B78" s="23"/>
       <c r="D78" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="22"/>
-      <c r="B79" s="22"/>
+      <c r="A79" s="23"/>
+      <c r="B79" s="23"/>
       <c r="D79" t="s">
         <v>48</v>
       </c>
@@ -11090,8 +11148,8 @@
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="22"/>
-      <c r="B80" s="22"/>
+      <c r="A80" s="23"/>
+      <c r="B80" s="23"/>
       <c r="D80" t="s">
         <v>81</v>
       </c>
@@ -11108,8 +11166,8 @@
       <c r="I80" s="5"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="22"/>
-      <c r="B81" s="22"/>
+      <c r="A81" s="23"/>
+      <c r="B81" s="23"/>
       <c r="D81" t="s">
         <v>202</v>
       </c>
@@ -11174,10 +11232,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>300</v>
       </c>
       <c r="C2" t="s">
@@ -11200,8 +11258,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="26"/>
       <c r="D3" t="s">
         <v>38</v>
       </c>
@@ -11219,8 +11277,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="26"/>
       <c r="D4" t="s">
         <v>40</v>
       </c>
@@ -11235,8 +11293,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="26"/>
       <c r="C5" t="s">
         <v>349</v>
       </c>
@@ -11245,8 +11303,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="25"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="26"/>
       <c r="D6" t="s">
         <v>48</v>
       </c>
@@ -11264,8 +11322,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="26"/>
       <c r="D7" t="s">
         <v>305</v>
       </c>
@@ -11281,8 +11339,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="26"/>
       <c r="C8" t="s">
         <v>351</v>
       </c>
@@ -11291,15 +11349,15 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="26"/>
       <c r="D9" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="26"/>
       <c r="D10" t="s">
         <v>48</v>
       </c>
@@ -11317,8 +11375,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="26"/>
       <c r="C11" t="s">
         <v>147</v>
       </c>
@@ -11327,8 +11385,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="26"/>
       <c r="D12" t="s">
         <v>152</v>
       </c>
@@ -11343,8 +11401,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="26"/>
       <c r="D13" t="s">
         <v>48</v>
       </c>
@@ -11362,8 +11420,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="26"/>
       <c r="D14" t="s">
         <v>154</v>
       </c>
@@ -11375,8 +11433,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="26"/>
       <c r="D15" t="s">
         <v>157</v>
       </c>
@@ -11388,8 +11446,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="26"/>
       <c r="D16" t="s">
         <v>159</v>
       </c>
@@ -11401,8 +11459,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="26"/>
       <c r="C17" t="s">
         <v>161</v>
       </c>
@@ -11411,8 +11469,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="26"/>
       <c r="D18" t="s">
         <v>159</v>
       </c>
@@ -11424,15 +11482,15 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="26"/>
       <c r="D19" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="25"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="26"/>
       <c r="D20" t="s">
         <v>152</v>
       </c>
@@ -11447,8 +11505,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="26"/>
       <c r="D21" t="s">
         <v>48</v>
       </c>
@@ -11466,8 +11524,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="25" t="s">
+      <c r="A22" s="23"/>
+      <c r="B22" s="26" t="s">
         <v>110</v>
       </c>
       <c r="C22" t="s">
@@ -11490,8 +11548,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="26"/>
       <c r="D23" t="s">
         <v>38</v>
       </c>
@@ -11509,8 +11567,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="25"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="26"/>
       <c r="D24" t="s">
         <v>40</v>
       </c>
@@ -11528,8 +11586,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="26"/>
       <c r="C25" t="s">
         <v>349</v>
       </c>
@@ -11538,8 +11596,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="25"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="26"/>
       <c r="D26" t="s">
         <v>48</v>
       </c>
@@ -11554,8 +11612,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="25"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="26"/>
       <c r="D27" t="s">
         <v>305</v>
       </c>
@@ -11568,8 +11626,8 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="26"/>
       <c r="C28" t="s">
         <v>355</v>
       </c>
@@ -11578,8 +11636,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="25"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="26"/>
       <c r="D29" t="s">
         <v>48</v>
       </c>
@@ -11597,8 +11655,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="25"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="26"/>
       <c r="C30" t="s">
         <v>161</v>
       </c>
@@ -11607,22 +11665,22 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="26"/>
       <c r="D31" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="25"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="26"/>
       <c r="D32" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="26"/>
       <c r="D33" t="s">
         <v>152</v>
       </c>
@@ -11637,8 +11695,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="25"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="26"/>
       <c r="D34" t="s">
         <v>48</v>
       </c>
@@ -11656,8 +11714,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22" t="s">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23" t="s">
         <v>101</v>
       </c>
       <c r="C35" t="s">
@@ -11680,8 +11738,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
       <c r="D36" t="s">
         <v>38</v>
       </c>
@@ -11699,8 +11757,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
       <c r="D37" t="s">
         <v>40</v>
       </c>
@@ -11718,8 +11776,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
       <c r="C38" t="s">
         <v>349</v>
       </c>
@@ -11728,8 +11786,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
       <c r="D39" t="s">
         <v>48</v>
       </c>
@@ -11744,8 +11802,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="23"/>
       <c r="D40" t="s">
         <v>305</v>
       </c>
@@ -11758,8 +11816,8 @@
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="23"/>
       <c r="C41" t="s">
         <v>350</v>
       </c>
@@ -11768,15 +11826,15 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="23"/>
       <c r="D42" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="D43" t="s">
         <v>48</v>
       </c>
@@ -11794,8 +11852,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" t="s">
         <v>147</v>
       </c>
@@ -11804,8 +11862,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="D45" t="s">
         <v>152</v>
       </c>
@@ -11820,8 +11878,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="D46" t="s">
         <v>48</v>
       </c>
@@ -11839,8 +11897,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="22"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
       <c r="D47" t="s">
         <v>154</v>
       </c>
@@ -11852,8 +11910,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="22"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
       <c r="D48" t="s">
         <v>157</v>
       </c>
@@ -11865,8 +11923,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="22"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
       <c r="D49" t="s">
         <v>159</v>
       </c>
@@ -11878,8 +11936,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="22"/>
+      <c r="A50" s="23"/>
+      <c r="B50" s="23"/>
       <c r="C50" t="s">
         <v>161</v>
       </c>
@@ -11888,8 +11946,8 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="22"/>
+      <c r="A51" s="23"/>
+      <c r="B51" s="23"/>
       <c r="D51" t="s">
         <v>159</v>
       </c>
@@ -11901,15 +11959,15 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="22"/>
+      <c r="A52" s="23"/>
+      <c r="B52" s="23"/>
       <c r="D52" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
+      <c r="A53" s="23"/>
+      <c r="B53" s="23"/>
       <c r="D53" t="s">
         <v>152</v>
       </c>
@@ -11924,8 +11982,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="22"/>
+      <c r="A54" s="23"/>
+      <c r="B54" s="23"/>
       <c r="D54" t="s">
         <v>48</v>
       </c>
@@ -11991,7 +12049,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>294</v>
       </c>
       <c r="B2" t="s">
@@ -12011,7 +12069,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="23"/>
       <c r="E3" t="s">
         <v>98</v>
       </c>
@@ -12020,7 +12078,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="E4" t="s">
         <v>101</v>
       </c>
@@ -12029,7 +12087,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" t="s">
         <v>102</v>
       </c>
@@ -12047,7 +12105,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="E6" t="s">
         <v>97</v>
       </c>
@@ -12056,7 +12114,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="E7" t="s">
         <v>101</v>
       </c>
@@ -12065,7 +12123,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" t="s">
         <v>106</v>
       </c>
@@ -12083,7 +12141,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="E9" t="s">
         <v>97</v>
       </c>
@@ -12092,7 +12150,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="E10" t="s">
         <v>101</v>
       </c>
@@ -12101,7 +12159,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="23" t="s">
         <v>295</v>
       </c>
       <c r="B11" t="s">
@@ -12121,7 +12179,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="E12" t="s">
         <v>110</v>
       </c>
@@ -12130,7 +12188,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="E13" t="s">
         <v>101</v>
       </c>
@@ -12139,7 +12197,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" t="s">
         <v>116</v>
       </c>
@@ -12157,7 +12215,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
+      <c r="A15" s="23"/>
       <c r="E15" t="s">
         <v>109</v>
       </c>
@@ -12166,7 +12224,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+      <c r="A16" s="23"/>
       <c r="E16" t="s">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
Fix some bugs, modify some codes
</commit_message>
<xml_diff>
--- a/dev/notes.xlsx
+++ b/dev/notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myLearning\lipGroup\riverGroup\integerateOmics\lipidPathways\newInspirationWork\procedure\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8FF067-FEF1-4165-AA35-98B99785B554}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8528F2A7-DCB2-4605-8149-119D052135E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{EE034DDF-90FE-4D0B-A13B-212579A2ECAA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{EE034DDF-90FE-4D0B-A13B-212579A2ECAA}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN function" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="973">
   <si>
     <t>Function</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3788,10 +3788,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>python3 getSplitWindowArgs.py -p "/home/lifs/temp/cor/" -k 8 -g 13 -o "/home/lifs/temp/cor/"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Yes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4078,10 +4074,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>circos图展示correlation绝对值大于改阈值的</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>展示富集到的前xx个GO term</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4249,31 +4241,61 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">Rscript lipVolcanoPlot.R -r "~/temp/" -s F -p "~/temp/results/" -b F -x "raw" -j 2 -k 0.1 -m 10 -w T </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Rscript correlation_main.R -i "./branch/benchmark/input/HANLipidMediator_imm_forcor.CSV" -d "./branch/benchmark/input/HANsampleList_lipmid.csv" -t "Metabolites" -l F -m 0.67 -j "./branch/benchmark/input/HANgene_tidy.CSV" -e "./branch/benchmark/input/HANsampleList.CSV" -u "RNAseq" -g 6 -k 4 -n F -s 0.4 -o "~/temp/cor_hi/" -b "hierarchical" -a "A"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Rscript correlation_main.R -i "./testData/SVFmultiomics_210118/input/lipids.csv" -d "./testData/SVFmultiomics_210118/input/sampleList.csv" -t "Lipids" -l T -m 0.67 -j "./testData/SVFmultiomics_210118/input/RNAseq_genesymbol.csv" -e "./testData/SVFmultiomics_210118/input/sampleList.csv" -u "RNAseq" -g 7 -k 6 -n T -o "~/temp/cor_kmeans/" -b "k_means"  -a "C"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Rscript correlation_main.R -i "./testData/SVFmultiomics_210118/input/metabolites.csv" -d "./testData/SVFmultiomics_210118/input/sampleList.csv" -t "Metabolites" -m 0.67 -j "./testData/SVFmultiomics_210118/input/RNAseq_genesymbol.csv" -e "./testData/SVFmultiomics_210118/input/sampleList.csv" -u "RNAseq" -c 4 -f 3 -n T -o "~/temp/cor_db/" -b "DBSCAN" -a "C"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Rscript correlation_main.R -i "./testData/CerebrospinalFluid_multiomics/input/metabolites_tidy2.csv" -d "./testData/CerebrospinalFluid_multiomics/input/sampleList_lip.csv" -t "Metabolites" -m 0.67 -j "./testData/CerebrospinalFluid_multiomics/input/proteins_Depletion_tidy.csv" -e "./testData/CerebrospinalFluid_multiomics/input/sampleList_lip.csv" -u "Proteins" -p 0.55 -n F -s 0.82 -o "~/temp/cor_mcl/" -b "MCL" -a "C"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Rscript lipVolcanoPlot.R -r "~/temp/" -s F -p "~/temp/results/" -b F -x "raw" -j 2 -k 0.1 -m 10 -w T </t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>circos图展示correlation绝对值大于该阈值的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>打印信息</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：Please check your correlation threshold. It may be too strict to filter.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>python3 getSplitWindowArgs.py -i "/home/lifs/temp/cor/" -o "/home/lifs/temp/cor/"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4379,6 +4401,44 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -4477,7 +4537,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4541,6 +4601,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="3" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4558,6 +4621,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="3" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="3" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4879,7 +4948,7 @@
   <dimension ref="A1:K87"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5080,7 +5149,7 @@
         <v>62</v>
       </c>
       <c r="K7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -5169,7 +5238,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>48</v>
       </c>
@@ -5189,31 +5258,30 @@
         <v>839</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="8" t="s">
+    <row r="13" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="15" t="s">
+        <v>951</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>953</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="G13" s="15" t="s">
+        <v>952</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>954</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="K13" s="15" t="s">
         <v>955</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>954</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>956</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>502</v>
       </c>
@@ -6705,8 +6773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0903CDAA-256C-4554-A139-C6A08F90034B}">
   <dimension ref="A1:J136"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6757,7 +6825,7 @@
     </row>
     <row r="2" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>486</v>
@@ -6766,16 +6834,16 @@
         <v>830</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>824</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="24" t="s">
         <v>828</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="15" t="s">
@@ -6784,9 +6852,9 @@
       <c r="F3" s="15" t="s">
         <v>825</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F4" s="14" t="s">
@@ -6796,7 +6864,7 @@
         <v>219</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -6827,7 +6895,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="F7" s="6" t="s">
         <v>237</v>
@@ -6840,7 +6908,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>485</v>
       </c>
@@ -6850,8 +6918,8 @@
       <c r="C8" s="15" t="s">
         <v>528</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>958</v>
+      <c r="D8" s="15" t="s">
+        <v>956</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>490</v>
@@ -6863,37 +6931,37 @@
       <c r="I8" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="J8" s="25" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="8" t="s">
-        <v>959</v>
+    <row r="9" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="15" t="s">
+        <v>957</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>945</v>
-      </c>
-      <c r="J9" s="24"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>943</v>
+      </c>
+      <c r="J9" s="25"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="D10" s="8" t="s">
-        <v>960</v>
+      <c r="D10" s="15" t="s">
+        <v>958</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="G10" s="15"/>
-      <c r="J10" s="24"/>
-    </row>
-    <row r="11" spans="1:10" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="25"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -6907,7 +6975,7 @@
       <c r="I11" s="6" t="s">
         <v>810</v>
       </c>
-      <c r="J11" s="24"/>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -6931,13 +6999,13 @@
       <c r="I12" t="s">
         <v>498</v>
       </c>
-      <c r="J12" s="24"/>
+      <c r="J12" s="25"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>496</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
@@ -6961,14 +7029,14 @@
       <c r="I14" t="s">
         <v>497</v>
       </c>
-      <c r="J14" s="24"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="F15" t="s">
         <v>653</v>
       </c>
-      <c r="J15" s="24"/>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
@@ -6981,7 +7049,7 @@
         <v>504</v>
       </c>
       <c r="D16" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F16" t="s">
         <v>233</v>
@@ -6992,14 +7060,14 @@
       <c r="I16" t="s">
         <v>497</v>
       </c>
-      <c r="J16" s="24"/>
+      <c r="J16" s="25"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="F17" t="s">
         <v>503</v>
       </c>
-      <c r="J17" s="24"/>
+      <c r="J17" s="25"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
@@ -7023,14 +7091,14 @@
       <c r="I18" t="s">
         <v>497</v>
       </c>
-      <c r="J18" s="24"/>
+      <c r="J18" s="25"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="F19" t="s">
         <v>508</v>
       </c>
-      <c r="J19" s="24"/>
+      <c r="J19" s="25"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
@@ -7054,14 +7122,14 @@
       <c r="I20" t="s">
         <v>497</v>
       </c>
-      <c r="J20" s="24"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="F21" t="s">
         <v>512</v>
       </c>
-      <c r="J21" s="24"/>
+      <c r="J21" s="25"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
@@ -7085,14 +7153,14 @@
       <c r="I22" t="s">
         <v>497</v>
       </c>
-      <c r="J22" s="24"/>
+      <c r="J22" s="25"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="F23" t="s">
         <v>669</v>
       </c>
-      <c r="J23" s="24"/>
+      <c r="J23" s="25"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
@@ -7116,13 +7184,13 @@
       <c r="I24" t="s">
         <v>497</v>
       </c>
-      <c r="J24" s="24"/>
+      <c r="J24" s="25"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>514</v>
       </c>
-      <c r="J25" s="24"/>
+      <c r="J25" s="25"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
@@ -7146,13 +7214,13 @@
       <c r="I26" t="s">
         <v>497</v>
       </c>
-      <c r="J26" s="24"/>
+      <c r="J26" s="25"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>681</v>
       </c>
-      <c r="J27" s="24"/>
+      <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -7205,7 +7273,7 @@
       <c r="I30" t="s">
         <v>694</v>
       </c>
-      <c r="J30" s="24" t="s">
+      <c r="J30" s="25" t="s">
         <v>585</v>
       </c>
     </row>
@@ -7219,7 +7287,7 @@
       <c r="I31" t="s">
         <v>516</v>
       </c>
-      <c r="J31" s="24"/>
+      <c r="J31" s="25"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
@@ -7231,7 +7299,7 @@
       <c r="I32" t="s">
         <v>122</v>
       </c>
-      <c r="J32" s="24"/>
+      <c r="J32" s="25"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
@@ -7243,7 +7311,7 @@
       <c r="I33" t="s">
         <v>536</v>
       </c>
-      <c r="J33" s="24"/>
+      <c r="J33" s="25"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F34" s="12" t="s">
@@ -7256,7 +7324,7 @@
       <c r="I34" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="J34" s="24"/>
+      <c r="J34" s="25"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F35" s="10" t="s">
@@ -7268,7 +7336,7 @@
       <c r="I35" t="s">
         <v>538</v>
       </c>
-      <c r="J35" s="24"/>
+      <c r="J35" s="25"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
@@ -7280,7 +7348,7 @@
       <c r="I36" t="s">
         <v>540</v>
       </c>
-      <c r="J36" s="24"/>
+      <c r="J36" s="25"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F37" s="6" t="s">
@@ -7293,7 +7361,7 @@
       <c r="I37" s="6" t="s">
         <v>810</v>
       </c>
-      <c r="J37" s="24"/>
+      <c r="J37" s="25"/>
     </row>
     <row r="38" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
@@ -7317,7 +7385,7 @@
       <c r="I38" t="s">
         <v>562</v>
       </c>
-      <c r="J38" s="24"/>
+      <c r="J38" s="25"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
@@ -7329,7 +7397,7 @@
       <c r="I39" t="s">
         <v>65</v>
       </c>
-      <c r="J39" s="24"/>
+      <c r="J39" s="25"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -7353,13 +7421,13 @@
       <c r="I40" t="s">
         <v>561</v>
       </c>
-      <c r="J40" s="24"/>
+      <c r="J40" s="25"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
         <v>576</v>
       </c>
-      <c r="J41" s="24"/>
+      <c r="J41" s="25"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -7383,13 +7451,13 @@
       <c r="I42" t="s">
         <v>561</v>
       </c>
-      <c r="J42" s="24"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F43" t="s">
         <v>579</v>
       </c>
-      <c r="J43" s="24"/>
+      <c r="J43" s="25"/>
     </row>
     <row r="44" spans="1:10" s="9" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
@@ -7453,7 +7521,7 @@
         <v>758</v>
       </c>
       <c r="I47" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -7810,81 +7878,81 @@
         <v>851</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="F71" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="G71" s="21" t="s">
-        <v>902</v>
-      </c>
-      <c r="H71" s="21"/>
-      <c r="I71" s="21"/>
+      <c r="G71" s="22" t="s">
+        <v>901</v>
+      </c>
+      <c r="H71" s="22"/>
+      <c r="I71" s="22"/>
     </row>
     <row r="72" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D72" s="13" t="s">
         <v>852</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="F72" s="15" t="s">
         <v>443</v>
       </c>
-      <c r="G72" s="22"/>
-      <c r="H72" s="22"/>
-      <c r="I72" s="22"/>
+      <c r="G72" s="23"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="23"/>
     </row>
     <row r="73" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D73" s="13" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="F73" s="15" t="s">
         <v>444</v>
       </c>
-      <c r="G73" s="22"/>
-      <c r="H73" s="22"/>
-      <c r="I73" s="22"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
     </row>
     <row r="74" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D74" s="13" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="F74" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="G74" s="22"/>
-      <c r="H74" s="22"/>
-      <c r="I74" s="22"/>
-    </row>
-    <row r="75" spans="1:10" s="15" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G74" s="23"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
+    </row>
+    <row r="75" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D75" s="13" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="F75" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="G75" s="23" t="s">
-        <v>903</v>
-      </c>
-      <c r="H75" s="23"/>
-      <c r="I75" s="23"/>
-    </row>
-    <row r="76" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D76" s="8" t="s">
-        <v>967</v>
+      <c r="G75" s="24" t="s">
+        <v>902</v>
+      </c>
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+    </row>
+    <row r="76" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D76" s="15" t="s">
+        <v>966</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="F76" s="15" t="s">
         <v>446</v>
@@ -7894,15 +7962,15 @@
       </c>
       <c r="H76" s="18"/>
       <c r="I76" s="18" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D77" s="8" t="s">
-        <v>968</v>
+        <v>899</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D77" s="15" t="s">
+        <v>967</v>
       </c>
       <c r="E77" s="15" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="F77" s="15" t="s">
         <v>447</v>
@@ -7912,15 +7980,15 @@
       </c>
       <c r="H77" s="18"/>
       <c r="I77" s="18" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D78" s="8" t="s">
-        <v>969</v>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D78" s="15" t="s">
+        <v>968</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="F78" s="15" t="s">
         <v>448</v>
@@ -7929,15 +7997,15 @@
         <v>219</v>
       </c>
       <c r="I78" s="15" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D79" s="8" t="s">
-        <v>970</v>
+        <v>898</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D79" s="15" t="s">
+        <v>969</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="F79" s="15" t="s">
         <v>449</v>
@@ -7949,10 +8017,10 @@
         <v>4</v>
       </c>
       <c r="I79" s="15" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" s="15" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F80" s="15" t="s">
         <v>408</v>
       </c>
@@ -7963,7 +8031,7 @@
         <v>4</v>
       </c>
       <c r="I80" s="15" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8007,21 +8075,21 @@
     </row>
     <row r="84" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F84" s="15" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="G84" s="15" t="s">
         <v>219</v>
       </c>
       <c r="H84" s="15" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="I84" s="15" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F85" s="15" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G85" s="15" t="s">
         <v>266</v>
@@ -8030,12 +8098,12 @@
         <v>4</v>
       </c>
       <c r="I85" s="15" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F86" s="15" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G86" s="15" t="s">
         <v>266</v>
@@ -8044,12 +8112,12 @@
         <v>3</v>
       </c>
       <c r="I86" s="15" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" s="15" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F87" s="15" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="G87" s="15" t="s">
         <v>322</v>
@@ -8058,24 +8126,24 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="I87" s="15" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F88" s="8" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="15" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F88" s="15" t="s">
+        <v>959</v>
+      </c>
+      <c r="G88" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="H88" s="15" t="s">
+        <v>960</v>
+      </c>
+      <c r="I88" s="15" t="s">
         <v>961</v>
       </c>
-      <c r="G88" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="H88" s="8" t="s">
-        <v>962</v>
-      </c>
-      <c r="I88" s="8" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" s="15" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:9" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="15" t="s">
         <v>462</v>
       </c>
@@ -8085,8 +8153,8 @@
       <c r="C89" s="15" t="s">
         <v>463</v>
       </c>
-      <c r="D89" s="15" t="s">
-        <v>858</v>
+      <c r="D89" s="8" t="s">
+        <v>972</v>
       </c>
       <c r="F89" s="15" t="s">
         <v>589</v>
@@ -8098,29 +8166,31 @@
         <v>856</v>
       </c>
     </row>
-    <row r="90" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F90" s="15" t="s">
+    <row r="90" spans="1:9" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F90" s="28" t="s">
         <v>592</v>
       </c>
-      <c r="G90" s="15" t="s">
+      <c r="G90" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="I90" s="15" t="s">
+      <c r="H90" s="29"/>
+      <c r="I90" s="29" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="91" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F91" s="15" t="s">
+    <row r="91" spans="1:9" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F91" s="29" t="s">
         <v>408</v>
       </c>
-      <c r="G91" s="15" t="s">
+      <c r="G91" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="I91" s="15" t="s">
+      <c r="H91" s="29"/>
+      <c r="I91" s="29" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" s="15" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="F92" s="6" t="s">
         <v>595</v>
       </c>
@@ -8140,7 +8210,7 @@
         <v>606</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D93" s="15" t="s">
         <v>613</v>
@@ -8157,7 +8227,7 @@
     </row>
     <row r="94" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D94" s="15" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="F94" s="15" t="s">
         <v>615</v>
@@ -8166,7 +8236,7 @@
         <v>596</v>
       </c>
       <c r="I94" s="15" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8177,7 +8247,7 @@
         <v>616</v>
       </c>
       <c r="I95" s="15" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8224,34 +8294,34 @@
         <v>65</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="100" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F100" s="6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>220</v>
       </c>
       <c r="H100" s="6"/>
       <c r="I100" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="J100" s="1"/>
     </row>
     <row r="101" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B101" s="15" t="s">
         <v>606</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D101" s="15" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="F101" s="15" t="s">
         <v>217</v>
@@ -8260,7 +8330,7 @@
         <v>219</v>
       </c>
       <c r="I101" s="15" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="102" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8271,7 +8341,7 @@
         <v>266</v>
       </c>
       <c r="I102" s="15" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="103" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8282,7 +8352,7 @@
         <v>219</v>
       </c>
       <c r="I103" s="15" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="104" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8318,59 +8388,59 @@
         <v>65</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="107" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F107" s="6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G107" s="6" t="s">
         <v>220</v>
       </c>
       <c r="H107" s="6"/>
       <c r="I107" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="J107" s="1"/>
     </row>
     <row r="108" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>606</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D108" s="15" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="F108" s="15" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="G108" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I108" s="15" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="109" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F109" s="15" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G109" s="15" t="s">
         <v>74</v>
       </c>
       <c r="I109" s="15" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="110" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F110" s="15" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="G110" s="15" t="s">
         <v>219</v>
@@ -8381,41 +8451,41 @@
     </row>
     <row r="111" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="15" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B111" s="15" t="s">
         <v>606</v>
       </c>
       <c r="C111" s="15" t="s">
+        <v>895</v>
+      </c>
+      <c r="D111" s="15" t="s">
         <v>896</v>
       </c>
-      <c r="D111" s="15" t="s">
-        <v>897</v>
-      </c>
       <c r="F111" s="15" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="G111" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I111" s="15" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="112" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F112" s="15" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G112" s="15" t="s">
         <v>74</v>
       </c>
       <c r="I112" s="15" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="113" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F113" s="15" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="G113" s="15" t="s">
         <v>219</v>
@@ -8424,41 +8494,41 @@
         <v>65</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="114" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B114" s="15" t="s">
         <v>850</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D114" s="15" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F114" s="15" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="G114" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I114" s="15" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="115" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F115" s="15" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="G115" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I115" s="15" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="116" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -8469,10 +8539,10 @@
         <v>266</v>
       </c>
       <c r="I116" s="15" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" s="15" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F117" s="15" t="s">
         <v>744</v>
       </c>
@@ -8480,26 +8550,29 @@
         <v>266</v>
       </c>
       <c r="I117" s="15" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" s="15" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F118" s="15" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G118" s="15" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="H118" s="15">
         <v>0.6</v>
       </c>
       <c r="I118" s="15" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>970</v>
+      </c>
+      <c r="J118" s="21" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" s="15" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="F119" s="15" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G119" s="15" t="s">
         <v>266</v>
@@ -8508,18 +8581,18 @@
         <v>20</v>
       </c>
       <c r="I119" s="15" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="120" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F120" s="15" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="G120" s="15" t="s">
         <v>219</v>
       </c>
       <c r="I120" s="15" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="121" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -8556,7 +8629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327B31EB-83BB-43B1-BAC3-91B270982CA0}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -8625,7 +8698,7 @@
       <c r="E3" t="s">
         <v>471</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="24" t="s">
         <v>706</v>
       </c>
     </row>
@@ -8642,7 +8715,7 @@
       <c r="E4" t="s">
         <v>472</v>
       </c>
-      <c r="F4" s="23"/>
+      <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -8657,7 +8730,7 @@
       <c r="E5" t="s">
         <v>473</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -8675,7 +8748,7 @@
       <c r="E6" t="s">
         <v>430</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="24" t="s">
         <v>705</v>
       </c>
       <c r="G6" t="s">
@@ -8698,7 +8771,7 @@
       <c r="E7" t="s">
         <v>655</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="24"/>
       <c r="G7" t="s">
         <v>713</v>
       </c>
@@ -8719,7 +8792,7 @@
       <c r="E8" t="s">
         <v>431</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="24" t="s">
         <v>700</v>
       </c>
     </row>
@@ -8737,7 +8810,7 @@
       <c r="E9" t="s">
         <v>432</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
@@ -8753,7 +8826,7 @@
       <c r="E10" t="s">
         <v>754</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -8771,7 +8844,7 @@
       <c r="E11" t="s">
         <v>399</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="24" t="s">
         <v>707</v>
       </c>
       <c r="G11" t="s">
@@ -8791,7 +8864,7 @@
       <c r="E12" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="F12" s="23"/>
+      <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -8806,7 +8879,7 @@
       <c r="E13" t="s">
         <v>465</v>
       </c>
-      <c r="F13" s="23"/>
+      <c r="F13" s="24"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -8821,7 +8894,7 @@
       <c r="E14" t="s">
         <v>482</v>
       </c>
-      <c r="F14" s="23"/>
+      <c r="F14" s="24"/>
       <c r="G14" t="s">
         <v>709</v>
       </c>
@@ -8839,7 +8912,7 @@
       <c r="E15" t="s">
         <v>401</v>
       </c>
-      <c r="F15" s="23"/>
+      <c r="F15" s="24"/>
       <c r="G15" t="s">
         <v>703</v>
       </c>
@@ -8860,7 +8933,7 @@
       <c r="E16" t="s">
         <v>672</v>
       </c>
-      <c r="F16" s="23"/>
+      <c r="F16" s="24"/>
       <c r="G16" t="s">
         <v>715</v>
       </c>
@@ -8884,7 +8957,7 @@
       <c r="E17" t="s">
         <v>403</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="24" t="s">
         <v>708</v>
       </c>
     </row>
@@ -8901,7 +8974,7 @@
       <c r="E18" t="s">
         <v>405</v>
       </c>
-      <c r="F18" s="23"/>
+      <c r="F18" s="24"/>
       <c r="G18" t="s">
         <v>701</v>
       </c>
@@ -8919,7 +8992,7 @@
       <c r="E19" t="s">
         <v>691</v>
       </c>
-      <c r="F19" s="23"/>
+      <c r="F19" s="24"/>
       <c r="G19" t="s">
         <v>700</v>
       </c>
@@ -8940,7 +9013,7 @@
       <c r="E20" t="s">
         <v>402</v>
       </c>
-      <c r="F20" s="23"/>
+      <c r="F20" s="24"/>
       <c r="G20" t="s">
         <v>703</v>
       </c>
@@ -8978,7 +9051,7 @@
       <c r="E22" t="s">
         <v>556</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="24" t="s">
         <v>817</v>
       </c>
     </row>
@@ -8995,7 +9068,7 @@
       <c r="E23" t="s">
         <v>553</v>
       </c>
-      <c r="F23" s="23"/>
+      <c r="F23" s="24"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="15" t="s">
@@ -9010,7 +9083,7 @@
       <c r="E24" t="s">
         <v>557</v>
       </c>
-      <c r="F24" s="23"/>
+      <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
@@ -9025,7 +9098,7 @@
       <c r="E25" t="s">
         <v>558</v>
       </c>
-      <c r="F25" s="23"/>
+      <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -9040,7 +9113,7 @@
       <c r="E26" t="s">
         <v>560</v>
       </c>
-      <c r="F26" s="23"/>
+      <c r="F26" s="24"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -9058,7 +9131,7 @@
       <c r="E27" t="s">
         <v>430</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="24" t="s">
         <v>816</v>
       </c>
     </row>
@@ -9075,7 +9148,7 @@
       <c r="E28" t="s">
         <v>570</v>
       </c>
-      <c r="F28" s="23"/>
+      <c r="F28" s="24"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -9133,7 +9206,7 @@
       <c r="E31" s="9" t="s">
         <v>610</v>
       </c>
-      <c r="F31" s="25" t="s">
+      <c r="F31" s="26" t="s">
         <v>742</v>
       </c>
       <c r="H31" s="9" t="s">
@@ -9153,7 +9226,7 @@
       <c r="E32" s="17" t="s">
         <v>792</v>
       </c>
-      <c r="F32" s="22"/>
+      <c r="F32" s="23"/>
     </row>
     <row r="33" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
@@ -9168,7 +9241,7 @@
       <c r="E33" s="17" t="s">
         <v>793</v>
       </c>
-      <c r="F33" s="22"/>
+      <c r="F33" s="23"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -9186,7 +9259,7 @@
       <c r="E34" s="14" t="s">
         <v>739</v>
       </c>
-      <c r="F34" s="23" t="s">
+      <c r="F34" s="24" t="s">
         <v>741</v>
       </c>
     </row>
@@ -9203,7 +9276,7 @@
       <c r="E35" s="14" t="s">
         <v>740</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="24"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -9221,7 +9294,7 @@
       <c r="E36" t="s">
         <v>641</v>
       </c>
-      <c r="F36" s="23"/>
+      <c r="F36" s="24"/>
       <c r="H36" t="s">
         <v>800</v>
       </c>
@@ -9239,7 +9312,7 @@
       <c r="E37" t="s">
         <v>642</v>
       </c>
-      <c r="F37" s="23"/>
+      <c r="F37" s="24"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -9254,7 +9327,7 @@
       <c r="E38" t="s">
         <v>643</v>
       </c>
-      <c r="F38" s="23"/>
+      <c r="F38" s="24"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -9272,7 +9345,7 @@
       <c r="E39" t="s">
         <v>774</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="F39" s="24" t="s">
         <v>772</v>
       </c>
     </row>
@@ -9289,7 +9362,7 @@
       <c r="E40" t="s">
         <v>775</v>
       </c>
-      <c r="F40" s="23"/>
+      <c r="F40" s="24"/>
       <c r="H40" s="15" t="s">
         <v>800</v>
       </c>
@@ -9307,7 +9380,7 @@
       <c r="E41" t="s">
         <v>776</v>
       </c>
-      <c r="F41" s="23"/>
+      <c r="F41" s="24"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
@@ -9322,7 +9395,7 @@
       <c r="E42" t="s">
         <v>777</v>
       </c>
-      <c r="F42" s="23"/>
+      <c r="F42" s="24"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="15" t="s">
@@ -9337,7 +9410,7 @@
       <c r="E43" t="s">
         <v>778</v>
       </c>
-      <c r="F43" s="23"/>
+      <c r="F43" s="24"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
@@ -9352,7 +9425,7 @@
       <c r="E44" t="s">
         <v>786</v>
       </c>
-      <c r="F44" s="23"/>
+      <c r="F44" s="24"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -9367,7 +9440,7 @@
       <c r="E45" t="s">
         <v>784</v>
       </c>
-      <c r="F45" s="23"/>
+      <c r="F45" s="24"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -9382,7 +9455,7 @@
       <c r="E46" t="s">
         <v>785</v>
       </c>
-      <c r="F46" s="23"/>
+      <c r="F46" s="24"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -9400,7 +9473,7 @@
       <c r="E47" t="s">
         <v>797</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="24" t="s">
         <v>836</v>
       </c>
     </row>
@@ -9417,7 +9490,7 @@
       <c r="E48" t="s">
         <v>798</v>
       </c>
-      <c r="F48" s="23"/>
+      <c r="F48" s="24"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -9435,7 +9508,7 @@
       <c r="E49" t="s">
         <v>807</v>
       </c>
-      <c r="F49" s="23"/>
+      <c r="F49" s="24"/>
       <c r="H49" s="15" t="s">
         <v>800</v>
       </c>
@@ -9448,7 +9521,7 @@
         <v>457</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>458</v>
@@ -9462,7 +9535,7 @@
         <v>460</v>
       </c>
       <c r="C51" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D51" t="s">
         <v>458</v>
@@ -9502,7 +9575,7 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
       <c r="B54" s="15" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>459</v>
@@ -9511,15 +9584,15 @@
         <v>458</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B55" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>400</v>
@@ -9528,15 +9601,15 @@
         <v>458</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B56" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C56" t="s">
         <v>400</v>
@@ -9545,15 +9618,15 @@
         <v>458</v>
       </c>
       <c r="E56" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B57" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C57" t="s">
         <v>459</v>
@@ -9562,12 +9635,12 @@
         <v>458</v>
       </c>
       <c r="E57" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C58" t="s">
         <v>400</v>
@@ -9576,15 +9649,15 @@
         <v>458</v>
       </c>
       <c r="E58" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
+        <v>890</v>
+      </c>
+      <c r="B59" t="s">
         <v>891</v>
-      </c>
-      <c r="B59" t="s">
-        <v>892</v>
       </c>
       <c r="C59" t="s">
         <v>400</v>
@@ -9593,12 +9666,12 @@
         <v>458</v>
       </c>
       <c r="E59" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C60" t="s">
         <v>459</v>
@@ -9607,12 +9680,12 @@
         <v>458</v>
       </c>
       <c r="E60" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C61" t="s">
         <v>459</v>
@@ -9621,7 +9694,7 @@
         <v>458</v>
       </c>
       <c r="E61" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="65" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -9891,7 +9964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66429DE9-DDD3-4C7B-9663-E821996E5CDF}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -9968,15 +10041,15 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C11" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
   </sheetData>
@@ -10005,10 +10078,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="B2" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -10088,10 +10161,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>94</v>
       </c>
       <c r="C2" t="s">
@@ -10117,8 +10190,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
       <c r="D3" t="s">
         <v>38</v>
       </c>
@@ -10139,8 +10212,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
       <c r="D4" t="s">
         <v>40</v>
       </c>
@@ -10152,8 +10225,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
       <c r="D5" t="s">
         <v>44</v>
       </c>
@@ -10174,8 +10247,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
       <c r="D6" t="s">
         <v>175</v>
       </c>
@@ -10193,8 +10266,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
       <c r="D7" t="s">
         <v>46</v>
       </c>
@@ -10211,8 +10284,8 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
       <c r="D8" t="s">
         <v>48</v>
       </c>
@@ -10233,8 +10306,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
       <c r="D9" t="s">
         <v>49</v>
       </c>
@@ -10246,8 +10319,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
       <c r="C10" t="s">
         <v>51</v>
       </c>
@@ -10256,8 +10329,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
       <c r="C11" t="s">
         <v>66</v>
       </c>
@@ -10266,15 +10339,15 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
       <c r="D12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
       <c r="D13" t="s">
         <v>48</v>
       </c>
@@ -10295,8 +10368,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
       <c r="C14" t="s">
         <v>69</v>
       </c>
@@ -10305,15 +10378,15 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
       <c r="D15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
       <c r="D16" t="s">
         <v>48</v>
       </c>
@@ -10334,8 +10407,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
       <c r="D17" t="s">
         <v>199</v>
       </c>
@@ -10356,8 +10429,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
       <c r="C18" t="s">
         <v>76</v>
       </c>
@@ -10366,15 +10439,15 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
       <c r="D19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
       <c r="D20" t="s">
         <v>48</v>
       </c>
@@ -10391,8 +10464,8 @@
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
       <c r="C21" t="s">
         <v>201</v>
       </c>
@@ -10401,15 +10474,15 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
       <c r="D22" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
       <c r="D23" t="s">
         <v>48</v>
       </c>
@@ -10426,8 +10499,8 @@
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
       <c r="D24" t="s">
         <v>81</v>
       </c>
@@ -10444,15 +10517,15 @@
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
       <c r="D25" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="26" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="27" t="s">
         <v>98</v>
       </c>
       <c r="C26" t="s">
@@ -10478,8 +10551,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="26"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="27"/>
       <c r="D27" t="s">
         <v>38</v>
       </c>
@@ -10500,8 +10573,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="27"/>
       <c r="D28" t="s">
         <v>40</v>
       </c>
@@ -10513,8 +10586,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="26"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="27"/>
       <c r="D29" t="s">
         <v>44</v>
       </c>
@@ -10535,8 +10608,8 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="26"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="27"/>
       <c r="D30" t="s">
         <v>45</v>
       </c>
@@ -10554,8 +10627,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="26"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="27"/>
       <c r="D31" t="s">
         <v>46</v>
       </c>
@@ -10572,8 +10645,8 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="26"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="27"/>
       <c r="D32" t="s">
         <v>48</v>
       </c>
@@ -10594,8 +10667,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="27"/>
       <c r="D33" t="s">
         <v>49</v>
       </c>
@@ -10607,8 +10680,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="26"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="27"/>
       <c r="C34" t="s">
         <v>51</v>
       </c>
@@ -10617,8 +10690,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="26"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="27"/>
       <c r="C35" t="s">
         <v>58</v>
       </c>
@@ -10627,15 +10700,15 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="26"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="27"/>
       <c r="D36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="27"/>
       <c r="D37" t="s">
         <v>61</v>
       </c>
@@ -10652,8 +10725,8 @@
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="27"/>
       <c r="D38" t="s">
         <v>48</v>
       </c>
@@ -10674,8 +10747,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="27"/>
       <c r="C39" t="s">
         <v>66</v>
       </c>
@@ -10684,15 +10757,15 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="27"/>
       <c r="D40" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="26"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="27"/>
       <c r="D41" t="s">
         <v>48</v>
       </c>
@@ -10713,8 +10786,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="26"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="27"/>
       <c r="C42" t="s">
         <v>69</v>
       </c>
@@ -10723,15 +10796,15 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="27"/>
       <c r="D43" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="27"/>
       <c r="D44" t="s">
         <v>48</v>
       </c>
@@ -10752,8 +10825,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="27"/>
       <c r="D45" t="s">
         <v>199</v>
       </c>
@@ -10774,8 +10847,8 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="27"/>
       <c r="C46" t="s">
         <v>76</v>
       </c>
@@ -10784,15 +10857,15 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="26"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="27"/>
       <c r="D47" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="26"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="27"/>
       <c r="D48" t="s">
         <v>48</v>
       </c>
@@ -10809,8 +10882,8 @@
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="26"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="27"/>
       <c r="C49" t="s">
         <v>201</v>
       </c>
@@ -10819,15 +10892,15 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="26"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="27"/>
       <c r="D50" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
-      <c r="B51" s="26"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="27"/>
       <c r="D51" t="s">
         <v>48</v>
       </c>
@@ -10844,8 +10917,8 @@
       <c r="I51" s="5"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="26"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="27"/>
       <c r="D52" t="s">
         <v>81</v>
       </c>
@@ -10862,15 +10935,15 @@
       <c r="I52" s="5"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="26"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="27"/>
       <c r="D53" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="23" t="s">
+      <c r="A54" s="24"/>
+      <c r="B54" s="24" t="s">
         <v>101</v>
       </c>
       <c r="C54" t="s">
@@ -10896,8 +10969,8 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="23"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="24"/>
       <c r="D55" t="s">
         <v>38</v>
       </c>
@@ -10918,8 +10991,8 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
-      <c r="B56" s="23"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="24"/>
       <c r="D56" t="s">
         <v>40</v>
       </c>
@@ -10931,8 +11004,8 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
-      <c r="B57" s="23"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="24"/>
       <c r="D57" t="s">
         <v>44</v>
       </c>
@@ -10953,8 +11026,8 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
-      <c r="B58" s="23"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="24"/>
       <c r="D58" t="s">
         <v>45</v>
       </c>
@@ -10972,8 +11045,8 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="23"/>
+      <c r="A59" s="24"/>
+      <c r="B59" s="24"/>
       <c r="D59" t="s">
         <v>46</v>
       </c>
@@ -10990,8 +11063,8 @@
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
+      <c r="A60" s="24"/>
+      <c r="B60" s="24"/>
       <c r="D60" t="s">
         <v>48</v>
       </c>
@@ -11012,8 +11085,8 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="23"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="24"/>
       <c r="D61" t="s">
         <v>49</v>
       </c>
@@ -11025,8 +11098,8 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
-      <c r="B62" s="23"/>
+      <c r="A62" s="24"/>
+      <c r="B62" s="24"/>
       <c r="C62" t="s">
         <v>51</v>
       </c>
@@ -11035,8 +11108,8 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
-      <c r="B63" s="23"/>
+      <c r="A63" s="24"/>
+      <c r="B63" s="24"/>
       <c r="C63" t="s">
         <v>58</v>
       </c>
@@ -11045,15 +11118,15 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="23"/>
+      <c r="A64" s="24"/>
+      <c r="B64" s="24"/>
       <c r="D64" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="23"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="24"/>
       <c r="D65" t="s">
         <v>61</v>
       </c>
@@ -11070,8 +11143,8 @@
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
-      <c r="B66" s="23"/>
+      <c r="A66" s="24"/>
+      <c r="B66" s="24"/>
       <c r="D66" t="s">
         <v>48</v>
       </c>
@@ -11092,8 +11165,8 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
-      <c r="B67" s="23"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="24"/>
       <c r="C67" t="s">
         <v>66</v>
       </c>
@@ -11102,15 +11175,15 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
-      <c r="B68" s="23"/>
+      <c r="A68" s="24"/>
+      <c r="B68" s="24"/>
       <c r="D68" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
-      <c r="B69" s="23"/>
+      <c r="A69" s="24"/>
+      <c r="B69" s="24"/>
       <c r="D69" t="s">
         <v>48</v>
       </c>
@@ -11131,8 +11204,8 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
-      <c r="B70" s="23"/>
+      <c r="A70" s="24"/>
+      <c r="B70" s="24"/>
       <c r="C70" t="s">
         <v>69</v>
       </c>
@@ -11141,15 +11214,15 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
-      <c r="B71" s="23"/>
+      <c r="A71" s="24"/>
+      <c r="B71" s="24"/>
       <c r="D71" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
-      <c r="B72" s="23"/>
+      <c r="A72" s="24"/>
+      <c r="B72" s="24"/>
       <c r="D72" t="s">
         <v>48</v>
       </c>
@@ -11170,8 +11243,8 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
-      <c r="B73" s="23"/>
+      <c r="A73" s="24"/>
+      <c r="B73" s="24"/>
       <c r="D73" t="s">
         <v>199</v>
       </c>
@@ -11192,8 +11265,8 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
-      <c r="B74" s="23"/>
+      <c r="A74" s="24"/>
+      <c r="B74" s="24"/>
       <c r="C74" t="s">
         <v>76</v>
       </c>
@@ -11202,15 +11275,15 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="B75" s="23"/>
+      <c r="A75" s="24"/>
+      <c r="B75" s="24"/>
       <c r="D75" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
-      <c r="B76" s="23"/>
+      <c r="A76" s="24"/>
+      <c r="B76" s="24"/>
       <c r="D76" t="s">
         <v>48</v>
       </c>
@@ -11227,8 +11300,8 @@
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
-      <c r="B77" s="23"/>
+      <c r="A77" s="24"/>
+      <c r="B77" s="24"/>
       <c r="C77" t="s">
         <v>201</v>
       </c>
@@ -11237,15 +11310,15 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
-      <c r="B78" s="23"/>
+      <c r="A78" s="24"/>
+      <c r="B78" s="24"/>
       <c r="D78" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="23"/>
-      <c r="B79" s="23"/>
+      <c r="A79" s="24"/>
+      <c r="B79" s="24"/>
       <c r="D79" t="s">
         <v>48</v>
       </c>
@@ -11262,8 +11335,8 @@
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
-      <c r="B80" s="23"/>
+      <c r="A80" s="24"/>
+      <c r="B80" s="24"/>
       <c r="D80" t="s">
         <v>81</v>
       </c>
@@ -11280,8 +11353,8 @@
       <c r="I80" s="5"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="23"/>
-      <c r="B81" s="23"/>
+      <c r="A81" s="24"/>
+      <c r="B81" s="24"/>
       <c r="D81" t="s">
         <v>202</v>
       </c>
@@ -11346,10 +11419,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>300</v>
       </c>
       <c r="C2" t="s">
@@ -11372,8 +11445,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="27"/>
       <c r="D3" t="s">
         <v>38</v>
       </c>
@@ -11391,8 +11464,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="27"/>
       <c r="D4" t="s">
         <v>40</v>
       </c>
@@ -11407,8 +11480,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="27"/>
       <c r="C5" t="s">
         <v>349</v>
       </c>
@@ -11417,8 +11490,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="27"/>
       <c r="D6" t="s">
         <v>48</v>
       </c>
@@ -11436,8 +11509,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="27"/>
       <c r="D7" t="s">
         <v>305</v>
       </c>
@@ -11453,8 +11526,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="27"/>
       <c r="C8" t="s">
         <v>351</v>
       </c>
@@ -11463,15 +11536,15 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="27"/>
       <c r="D9" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="27"/>
       <c r="D10" t="s">
         <v>48</v>
       </c>
@@ -11489,8 +11562,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="27"/>
       <c r="C11" t="s">
         <v>147</v>
       </c>
@@ -11499,8 +11572,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="27"/>
       <c r="D12" t="s">
         <v>152</v>
       </c>
@@ -11515,8 +11588,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="27"/>
       <c r="D13" t="s">
         <v>48</v>
       </c>
@@ -11534,8 +11607,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="27"/>
       <c r="D14" t="s">
         <v>154</v>
       </c>
@@ -11547,8 +11620,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="27"/>
       <c r="D15" t="s">
         <v>157</v>
       </c>
@@ -11560,8 +11633,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="27"/>
       <c r="D16" t="s">
         <v>159</v>
       </c>
@@ -11573,8 +11646,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="27"/>
       <c r="C17" t="s">
         <v>161</v>
       </c>
@@ -11583,8 +11656,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="27"/>
       <c r="D18" t="s">
         <v>159</v>
       </c>
@@ -11596,15 +11669,15 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="27"/>
       <c r="D19" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="27"/>
       <c r="D20" t="s">
         <v>152</v>
       </c>
@@ -11619,8 +11692,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="26"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="27"/>
       <c r="D21" t="s">
         <v>48</v>
       </c>
@@ -11638,8 +11711,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="26" t="s">
+      <c r="A22" s="24"/>
+      <c r="B22" s="27" t="s">
         <v>110</v>
       </c>
       <c r="C22" t="s">
@@ -11662,8 +11735,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="27"/>
       <c r="D23" t="s">
         <v>38</v>
       </c>
@@ -11681,8 +11754,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="27"/>
       <c r="D24" t="s">
         <v>40</v>
       </c>
@@ -11700,8 +11773,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="26"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="27"/>
       <c r="C25" t="s">
         <v>349</v>
       </c>
@@ -11710,8 +11783,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="27"/>
       <c r="D26" t="s">
         <v>48</v>
       </c>
@@ -11726,8 +11799,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="26"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="27"/>
       <c r="D27" t="s">
         <v>305</v>
       </c>
@@ -11740,8 +11813,8 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="27"/>
       <c r="C28" t="s">
         <v>355</v>
       </c>
@@ -11750,8 +11823,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="26"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="27"/>
       <c r="D29" t="s">
         <v>48</v>
       </c>
@@ -11769,8 +11842,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="26"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="27"/>
       <c r="C30" t="s">
         <v>161</v>
       </c>
@@ -11779,22 +11852,22 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="26"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="27"/>
       <c r="D31" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="26"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="27"/>
       <c r="D32" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="27"/>
       <c r="D33" t="s">
         <v>152</v>
       </c>
@@ -11809,8 +11882,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="26"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="27"/>
       <c r="D34" t="s">
         <v>48</v>
       </c>
@@ -11828,8 +11901,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23" t="s">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24" t="s">
         <v>101</v>
       </c>
       <c r="C35" t="s">
@@ -11852,8 +11925,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="24"/>
       <c r="D36" t="s">
         <v>38</v>
       </c>
@@ -11871,8 +11944,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="24"/>
       <c r="D37" t="s">
         <v>40</v>
       </c>
@@ -11890,8 +11963,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
       <c r="C38" t="s">
         <v>349</v>
       </c>
@@ -11900,8 +11973,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="24"/>
       <c r="D39" t="s">
         <v>48</v>
       </c>
@@ -11916,8 +11989,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
       <c r="D40" t="s">
         <v>305</v>
       </c>
@@ -11930,8 +12003,8 @@
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
       <c r="C41" t="s">
         <v>350</v>
       </c>
@@ -11940,15 +12013,15 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
       <c r="D42" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="24"/>
       <c r="D43" t="s">
         <v>48</v>
       </c>
@@ -11966,8 +12039,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
       <c r="C44" t="s">
         <v>147</v>
       </c>
@@ -11976,8 +12049,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
       <c r="D45" t="s">
         <v>152</v>
       </c>
@@ -11992,8 +12065,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="24"/>
       <c r="D46" t="s">
         <v>48</v>
       </c>
@@ -12011,8 +12084,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="23"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="24"/>
       <c r="D47" t="s">
         <v>154</v>
       </c>
@@ -12024,8 +12097,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="23"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="24"/>
       <c r="D48" t="s">
         <v>157</v>
       </c>
@@ -12037,8 +12110,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="23"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="24"/>
       <c r="D49" t="s">
         <v>159</v>
       </c>
@@ -12050,8 +12123,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="23"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="24"/>
       <c r="C50" t="s">
         <v>161</v>
       </c>
@@ -12060,8 +12133,8 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
-      <c r="B51" s="23"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="24"/>
       <c r="D51" t="s">
         <v>159</v>
       </c>
@@ -12073,15 +12146,15 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="23"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="24"/>
       <c r="D52" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="23"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="24"/>
       <c r="D53" t="s">
         <v>152</v>
       </c>
@@ -12096,8 +12169,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="23"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="24"/>
       <c r="D54" t="s">
         <v>48</v>
       </c>
@@ -12163,7 +12236,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>294</v>
       </c>
       <c r="B2" t="s">
@@ -12183,7 +12256,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="24"/>
       <c r="E3" t="s">
         <v>98</v>
       </c>
@@ -12192,7 +12265,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="E4" t="s">
         <v>101</v>
       </c>
@@ -12201,7 +12274,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" t="s">
         <v>102</v>
       </c>
@@ -12219,7 +12292,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="E6" t="s">
         <v>97</v>
       </c>
@@ -12228,7 +12301,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="E7" t="s">
         <v>101</v>
       </c>
@@ -12237,7 +12310,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" t="s">
         <v>106</v>
       </c>
@@ -12255,7 +12328,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="E9" t="s">
         <v>97</v>
       </c>
@@ -12264,7 +12337,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="E10" t="s">
         <v>101</v>
       </c>
@@ -12273,7 +12346,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>295</v>
       </c>
       <c r="B11" t="s">
@@ -12293,7 +12366,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="E12" t="s">
         <v>110</v>
       </c>
@@ -12302,7 +12375,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="E13" t="s">
         <v>101</v>
       </c>
@@ -12311,7 +12384,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" t="s">
         <v>116</v>
       </c>
@@ -12329,7 +12402,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="E15" t="s">
         <v>109</v>
       </c>
@@ -12338,7 +12411,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="E16" t="s">
         <v>101</v>
       </c>

</xml_diff>